<commit_message>
Change requirements and gitignore
</commit_message>
<xml_diff>
--- a/custom-app.xlsx
+++ b/custom-app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Documents\DEV\Python\qradar-qid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30A589B-FF2E-4DC2-976E-640D207F428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5F2BA-0D7B-418D-A5A4-FD76A4C71E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{2DD3A2D9-C40A-4D9C-9006-194803CABA20}"/>
+    <workbookView xWindow="4200" yWindow="-13365" windowWidth="17280" windowHeight="8880" xr2:uid="{2DD3A2D9-C40A-4D9C-9006-194803CABA20}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -908,17 +908,18 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D51"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -932,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -946,7 +947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -960,7 +961,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -974,7 +975,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -988,7 +989,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1114,7 +1115,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1226,7 +1227,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1436,7 +1437,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1506,7 +1507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1639,15 +1640,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A191DC8596FFBA44A8B41E275F813DCD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d007381e99add0abe42ba597c0f02292">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="add094fb-889f-429c-ae29-e490a80ce16f" xmlns:ns4="853af9c1-f245-4859-8f8d-b02793badbc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f913c8e78810ad845daadd60bee39f6a" ns3:_="" ns4:_="">
     <xsd:import namespace="add094fb-889f-429c-ae29-e490a80ce16f"/>
@@ -1868,6 +1860,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1877,14 +1878,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA5EFBB7-DC15-4989-95B9-D8F7BFCAB715}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02C474A0-6288-44F3-B53A-482C05A548D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1899,6 +1892,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA5EFBB7-DC15-4989-95B9-D8F7BFCAB715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>